<commit_message>
Fix export data and money graph
</commit_message>
<xml_diff>
--- a/countries_weather_data.xlsx
+++ b/countries_weather_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,11 +457,6 @@
           <t>windspeeds</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>currency_group</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -490,15 +485,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>25.2</v>
+        <v>21.4</v>
       </c>
       <c r="G2" t="n">
-        <v>16</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Pesos</t>
-        </is>
+        <v>13.8</v>
       </c>
     </row>
     <row r="3">
@@ -528,15 +518,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>31.1</v>
+        <v>29.3</v>
       </c>
       <c r="G3" t="n">
-        <v>20.6</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Pesos</t>
-        </is>
+        <v>14.8</v>
       </c>
     </row>
     <row r="4">
@@ -566,15 +551,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>30.5</v>
+        <v>30.1</v>
       </c>
       <c r="G4" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+        <v>5.9</v>
       </c>
     </row>
     <row r="5">
@@ -604,15 +584,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>12.3</v>
+        <v>12.8</v>
       </c>
       <c r="G5" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+        <v>8.4</v>
       </c>
     </row>
     <row r="6">
@@ -642,15 +617,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>25.4</v>
+        <v>24</v>
       </c>
       <c r="G6" t="n">
-        <v>15.1</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Pesos</t>
-        </is>
+        <v>12.2</v>
       </c>
     </row>
     <row r="7">
@@ -680,15 +650,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>30.2</v>
+        <v>28.9</v>
       </c>
       <c r="G7" t="n">
-        <v>13.8</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Dólares</t>
-        </is>
+        <v>7.1</v>
       </c>
     </row>
     <row r="8">
@@ -718,15 +683,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>15.2</v>
+        <v>17.2</v>
       </c>
       <c r="G8" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+        <v>6.8</v>
       </c>
     </row>
     <row r="9">
@@ -756,15 +716,10 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>34.5</v>
+        <v>32.9</v>
       </c>
       <c r="G9" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+        <v>7.9</v>
       </c>
     </row>
     <row r="10">
@@ -794,15 +749,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>37.5</v>
+        <v>36.3</v>
       </c>
       <c r="G10" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Pesos</t>
-        </is>
+        <v>21.1</v>
       </c>
     </row>
     <row r="11">
@@ -832,15 +782,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>33.5</v>
+        <v>30.3</v>
       </c>
       <c r="G11" t="n">
-        <v>27.9</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+        <v>31.3</v>
       </c>
     </row>
     <row r="12">
@@ -870,15 +815,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>6</v>
+        <v>10.9</v>
       </c>
       <c r="G12" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
@@ -908,15 +848,10 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-0.4</v>
+        <v>-0</v>
       </c>
       <c r="G13" t="n">
-        <v>23.1</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>7.2</v>
       </c>
     </row>
     <row r="14">
@@ -946,15 +881,10 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>6.7</v>
+        <v>7.5</v>
       </c>
       <c r="G14" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>6.9</v>
       </c>
     </row>
     <row r="15">
@@ -984,15 +914,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>9.9</v>
+        <v>12.6</v>
       </c>
       <c r="G15" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>37.5</v>
       </c>
     </row>
     <row r="16">
@@ -1022,15 +947,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>12.5</v>
+        <v>13.2</v>
       </c>
       <c r="G16" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>23.8</v>
       </c>
     </row>
     <row r="17">
@@ -1060,16 +980,11 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>26.2</v>
+        <v>26.4</v>
       </c>
       <c r="G17" t="n">
         <v>33.7</v>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Dólares</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1098,15 +1013,10 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>8.800000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="G18" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>12.2</v>
       </c>
     </row>
     <row r="19">
@@ -1136,15 +1046,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.2</v>
+        <v>3.3</v>
       </c>
       <c r="G19" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+        <v>1.3</v>
       </c>
     </row>
     <row r="20">
@@ -1174,15 +1079,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0.1</v>
+        <v>1.7</v>
       </c>
       <c r="G20" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>0.7</v>
       </c>
     </row>
     <row r="21">
@@ -1212,15 +1112,10 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>8.6</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Euros</t>
-        </is>
+        <v>2.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>